<commit_message>
Push to Master various practices
</commit_message>
<xml_diff>
--- a/GmailProject/testData/gmail.xlsx
+++ b/GmailProject/testData/gmail.xlsx
@@ -14,22 +14,15 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Tester, welcome to your new Google Account</t>
+    <t>Critical security alert</t>
   </si>
   <si>
-    <t>Hi Tester,
-Thank you for creating a Google Account. Here is some advice to get started with your Google account.
-You're in control
-Choose what's right for you. Manage your privacy and security settings at any time in your Google Account, where you can sign up for Privacy Checkup reminders, take the Security Checkup and more.
-Access Gmail on the go
-With Gmail for Android or iOS, you get one click access to your email, real-time notifications and a lot more wherever you are.
-Discover Google products
-Find tips to use other Google products here. For example, Google Photos for Android or iOS gives you free photo and video storage on your phone.
-Replies to this email aren't monitored, but if you have a question try the Help Center or post it to the Gmail Help Forum where my team and other expert users answer questions.
-Enjoy your new account,
-Google Community Team
-© 2020 Google Ireland Ltd, Gordon House, Barrow Street, Dublin 4, Ireland.
-This email was sent to you because you created a Google Account.</t>
+    <t>Sign-in attempt was blocked
+mailfortesting086@gmail.com
+Someone just used your password to try to sign in to your account. Google blocked them, but you should check what happened.
+Check activity
+You received this email to let you know about important changes to your Google Account and services.
+© 2020 Google LLC, 1600 Amphitheatre Parkway, Mountain View, CA 94043, USA</t>
   </si>
 </sst>
 </file>

</xml_diff>